<commit_message>
Last version up to date
</commit_message>
<xml_diff>
--- a/Documents/ProjectExpenses.xlsx
+++ b/Documents/ProjectExpenses.xlsx
@@ -14,14 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="54">
   <si>
     <t>Лице</t>
   </si>
   <si>
-    <t>Ставка</t>
-  </si>
-  <si>
     <t>Дата</t>
   </si>
   <si>
@@ -122,6 +119,63 @@
   </si>
   <si>
     <t>Работа по изграждането на дървовидната структура на организацията</t>
+  </si>
+  <si>
+    <t>Завършени длъжности в организацията</t>
+  </si>
+  <si>
+    <t>Завършена дървоводната структура</t>
+  </si>
+  <si>
+    <t>Прихванати ситуации при изтриване на обекти - издава подходящо съобщение за грешка, когато изтриването е недопустимо.</t>
+  </si>
+  <si>
+    <t>Контекстни менюта в структрата на организацията за разместване на дървиводната структура и за разместване на реда на длъжностите в структурата.</t>
+  </si>
+  <si>
+    <t>Реализиран прозореца за визуализация на картотеката и заявките за избор на лица</t>
+  </si>
+  <si>
+    <t>Доработени длъжности, звена и длъжности в организацията да имат дата на валидност</t>
+  </si>
+  <si>
+    <t>Проектирани класификатори по НКПД и ЕКАТТЕ с автоматичен импорт. Реализация - за HR модула, ако има такъв.</t>
+  </si>
+  <si>
+    <t>Работа по реализацията на прозореца за висуализация и редакция на лични данни и данни за назначения.</t>
+  </si>
+  <si>
+    <t>Проучване на начини за реализация на одит лог</t>
+  </si>
+  <si>
+    <t>Реализация на одит лог</t>
+  </si>
+  <si>
+    <t>Проектиране на функционалност за екипи, членове на екипи, коли на екипи, всички различни видове графици (дневен, месечен, шестмесечен, присъствена форма)</t>
+  </si>
+  <si>
+    <t>Проектиране на потребителски контроли за прозорците на досието</t>
+  </si>
+  <si>
+    <t>Изчистване на проблеми в архитектурата бизнес логиката</t>
+  </si>
+  <si>
+    <t>Изчистване на проблеми в архитектурата на базата данни</t>
+  </si>
+  <si>
+    <t>Въвеждане на структурата на организацията</t>
+  </si>
+  <si>
+    <t>Изчистване на проблеми в архитектурата бизнес логиката - приключени</t>
+  </si>
+  <si>
+    <t>Импорт на данни за длъжностите в организацията</t>
+  </si>
+  <si>
+    <t>Импорт на данни за длъжностите в структурата на организацията</t>
+  </si>
+  <si>
+    <t>Подготовка на данните от щатното разписание за импорт</t>
   </si>
 </sst>
 </file>
@@ -494,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M45"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,38 +565,32 @@
     <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>12.201499999999999</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2">
         <v>2</v>
@@ -551,21 +599,21 @@
         <v>100</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2">
         <v>2000</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>12.201499999999999</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
@@ -574,21 +622,21 @@
         <v>100</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H3">
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1.2016</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2">
         <v>2</v>
@@ -597,21 +645,21 @@
         <v>100</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H4">
         <v>2400</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1.2016</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2">
         <v>2</v>
@@ -620,21 +668,21 @@
         <v>100</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H5">
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1.2016</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2">
         <v>3</v>
@@ -643,15 +691,15 @@
         <v>300</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>1.2016</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2">
         <v>6</v>
@@ -660,22 +708,22 @@
         <v>300</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H7">
         <f>SUM(H2:H6)</f>
         <v>5600</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>42380</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -684,15 +732,15 @@
         <v>150</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>42381</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" s="2">
         <v>2</v>
@@ -701,15 +749,15 @@
         <v>100</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>42381</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="2">
         <v>2</v>
@@ -718,15 +766,15 @@
         <v>100</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>42383</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" s="2">
         <v>2</v>
@@ -735,15 +783,15 @@
         <v>100</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>42384</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="2">
         <v>4</v>
@@ -752,15 +800,15 @@
         <v>200</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>42387</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13" s="2">
         <v>4</v>
@@ -769,15 +817,15 @@
         <v>200</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>42387</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" s="2">
         <v>1</v>
@@ -786,15 +834,15 @@
         <v>50</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>42387</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="2">
         <v>1</v>
@@ -803,24 +851,24 @@
         <v>50</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>42388</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2">
+        <v>50</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="C16" s="2">
-        <v>1</v>
-      </c>
-      <c r="D16" s="2">
-        <v>50</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -828,7 +876,7 @@
         <v>42389</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" s="2">
         <v>2</v>
@@ -837,7 +885,7 @@
         <v>100</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -845,7 +893,7 @@
         <v>42389</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18" s="2">
         <v>1</v>
@@ -854,7 +902,7 @@
         <v>50</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -862,7 +910,7 @@
         <v>42389</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19" s="2">
         <v>0.5</v>
@@ -871,7 +919,7 @@
         <v>25</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -879,7 +927,7 @@
         <v>42390</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20" s="2">
         <v>2</v>
@@ -888,7 +936,7 @@
         <v>100</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -896,7 +944,7 @@
         <v>42390</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" s="2">
         <v>2</v>
@@ -905,7 +953,7 @@
         <v>100</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -913,7 +961,7 @@
         <v>42390</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22" s="2">
         <v>1</v>
@@ -922,7 +970,7 @@
         <v>50</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -930,7 +978,7 @@
         <v>42390</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" s="2">
         <v>1</v>
@@ -939,7 +987,7 @@
         <v>50</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -947,7 +995,7 @@
         <v>42391</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24" s="2">
         <v>1</v>
@@ -956,7 +1004,7 @@
         <v>50</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="105" x14ac:dyDescent="0.25">
@@ -964,7 +1012,7 @@
         <v>42392</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C25" s="2">
         <v>4</v>
@@ -973,7 +1021,7 @@
         <v>200</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -981,7 +1029,7 @@
         <v>42393</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C26" s="2">
         <v>1</v>
@@ -990,7 +1038,7 @@
         <v>50</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -998,7 +1046,7 @@
         <v>42393</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C27" s="2">
         <v>2</v>
@@ -1007,137 +1055,411 @@
         <v>100</v>
       </c>
       <c r="E27" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>42394</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1</v>
+      </c>
+      <c r="D28" s="2">
+        <v>50</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>42395</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1</v>
+      </c>
+      <c r="D29" s="2">
+        <v>50</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
+    <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>42396</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1</v>
+      </c>
+      <c r="D30" s="2">
+        <v>50</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>42396</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="2">
+        <v>1</v>
+      </c>
+      <c r="D31" s="2">
+        <v>50</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>42406</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="2">
+        <v>1</v>
+      </c>
+      <c r="D32" s="2">
+        <v>50</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>42406</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="2">
+        <v>1</v>
+      </c>
+      <c r="D33" s="2">
+        <v>50</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>42407</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="2">
+        <v>2</v>
+      </c>
+      <c r="D34" s="2">
+        <v>100</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>42407</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="2">
+        <v>1</v>
+      </c>
+      <c r="D35" s="2">
+        <v>50</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
+      <c r="A36" s="1">
+        <v>42411</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="2">
+        <v>1</v>
+      </c>
+      <c r="D36" s="2">
+        <v>50</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
+      <c r="A37" s="1">
+        <v>42412</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="2">
+        <v>2</v>
+      </c>
+      <c r="D37" s="2">
+        <v>100</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>42412</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="2">
+        <v>6</v>
+      </c>
+      <c r="D38" s="2">
+        <v>300</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>42416</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="2">
+        <v>1</v>
+      </c>
+      <c r="D39" s="2">
+        <v>50</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>42417</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="2">
+        <v>1</v>
+      </c>
+      <c r="D40" s="2">
+        <v>50</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>42418</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="2">
+        <v>1</v>
+      </c>
+      <c r="D41" s="2">
+        <v>50</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
+      <c r="A42" s="1">
+        <v>42418</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" s="2">
+        <v>1</v>
+      </c>
+      <c r="D42" s="2">
+        <v>50</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>42418</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" s="2">
+        <v>1</v>
+      </c>
+      <c r="D43" s="2">
+        <v>50</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-    </row>
-    <row r="45" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A45" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="3">
-        <f>SUM(D2:D28)</f>
-        <v>2875</v>
+      <c r="A44" s="1">
+        <v>42418</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D44" s="2">
+        <v>25</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>42418</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D45" s="2">
+        <v>25</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>42419</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="2">
+        <v>2</v>
+      </c>
+      <c r="D46" s="2">
+        <v>100</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+    </row>
+    <row r="57" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A57" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="3">
+        <f>SUM(D2:D46)</f>
+        <v>4175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Last changes working in CSMP
</commit_message>
<xml_diff>
--- a/Documents/ProjectExpenses.xlsx
+++ b/Documents/ProjectExpenses.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="99">
   <si>
     <t>Лице</t>
   </si>
@@ -272,6 +272,45 @@
   </si>
   <si>
     <t>Създадена таблицата в базата данни за графиците</t>
+  </si>
+  <si>
+    <t>Реализиран интерфейс за отпуски на служител, и полагаем годишен отпуск.</t>
+  </si>
+  <si>
+    <t>Добавени годишни отпуски за всички служители.</t>
+  </si>
+  <si>
+    <t>Проектиране на визуализациите на видовете графици, номенклатура на видовете графици и генерация на графиците</t>
+  </si>
+  <si>
+    <t>Реализация на номенклатура за видове графици</t>
+  </si>
+  <si>
+    <t>Реализация на визуализацията на екипи съчетани с графици, филтър по дата и по вид график</t>
+  </si>
+  <si>
+    <t>Реализация на нова логика за бързо визуализиране на графиците и екипите в организацията</t>
+  </si>
+  <si>
+    <t>Реализация на нов потребителски интерфейс за бързо визуализиране на графиците и екипите в организацията.</t>
+  </si>
+  <si>
+    <t>Добавени полетата ТРЗ код и Графици код</t>
+  </si>
+  <si>
+    <t>Довършено генерирането на графици с правилна формула</t>
+  </si>
+  <si>
+    <t>Реализация на потребителски интерфейс за генериране на графиците. Тестване на логиката на генерираенто, чистене на проблеми, разписана логика за запаметяване на графици.</t>
+  </si>
+  <si>
+    <t>Реализация на логиката за генериране на графици, вмъкване на отпуските в графиците</t>
+  </si>
+  <si>
+    <t>Добавено описание на редовете въф формата за работни дни през месеца.</t>
+  </si>
+  <si>
+    <t>Генерация на графици.</t>
   </si>
 </sst>
 </file>
@@ -648,15 +687,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N74"/>
+  <dimension ref="A1:N88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="8" customWidth="1"/>
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" customWidth="1"/>
@@ -1954,50 +1993,252 @@
         <v>85</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
+    <row r="69" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>42443</v>
+      </c>
       <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
-      <c r="E69" s="2"/>
+      <c r="C69" s="2">
+        <v>3</v>
+      </c>
+      <c r="D69" s="2">
+        <v>150</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
+      <c r="A70" s="1">
+        <v>42443</v>
+      </c>
       <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
+      <c r="C70" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D70" s="2">
+        <v>25</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>42444</v>
+      </c>
       <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
-      <c r="D71" s="2"/>
-      <c r="E71" s="2"/>
+      <c r="C71" s="2">
+        <v>2</v>
+      </c>
+      <c r="D71" s="2">
+        <v>50</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
+      <c r="A72" s="1">
+        <v>42444</v>
+      </c>
       <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
-      <c r="E72" s="2"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
+      <c r="C72" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D72" s="2">
+        <v>25</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>42444</v>
+      </c>
       <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2"/>
-    </row>
-    <row r="74" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A74" s="3" t="s">
+      <c r="C73" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="D73" s="2">
+        <v>75</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>42445</v>
+      </c>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2">
+        <v>4</v>
+      </c>
+      <c r="D74" s="2">
+        <v>200</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>42446</v>
+      </c>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2">
+        <v>3</v>
+      </c>
+      <c r="D75" s="2">
+        <v>150</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>42447</v>
+      </c>
+      <c r="B76" s="2"/>
+      <c r="C76" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D76" s="2">
+        <v>25</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>42447</v>
+      </c>
+      <c r="B77" s="2"/>
+      <c r="C77" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="D77" s="2">
+        <v>75</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>42447</v>
+      </c>
+      <c r="B78" s="2"/>
+      <c r="C78" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D78" s="2">
+        <v>25</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>42448</v>
+      </c>
+      <c r="B79" s="2"/>
+      <c r="C79" s="2">
+        <v>2</v>
+      </c>
+      <c r="D79" s="2">
+        <v>100</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>42448</v>
+      </c>
+      <c r="B80" s="2"/>
+      <c r="C80" s="2">
+        <v>2</v>
+      </c>
+      <c r="D80" s="2">
+        <v>100</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>42450</v>
+      </c>
+      <c r="B81" s="2"/>
+      <c r="C81" s="2">
+        <v>4</v>
+      </c>
+      <c r="D81" s="2">
+        <v>200</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="1"/>
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="1"/>
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="1"/>
+      <c r="B84" s="2"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="1"/>
+      <c r="B85" s="2"/>
+      <c r="C85" s="2"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="1"/>
+      <c r="B86" s="2"/>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="1"/>
+      <c r="B87" s="2"/>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+    </row>
+    <row r="88" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A88" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B74" s="4"/>
-      <c r="C74" s="4"/>
-      <c r="D74" s="3">
-        <f>SUM(D2:D68)</f>
-        <v>4750</v>
+      <c r="B88" s="4"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="3">
+        <f>SUM(D2:D81)</f>
+        <v>5950</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working single department schedule generation
</commit_message>
<xml_diff>
--- a/Documents/ProjectExpenses.xlsx
+++ b/Documents/ProjectExpenses.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="103">
   <si>
     <t>Лице</t>
   </si>
@@ -311,6 +311,18 @@
   </si>
   <si>
     <t>Генерация на графици.</t>
+  </si>
+  <si>
+    <t>Внедряване и доработки на място</t>
+  </si>
+  <si>
+    <t>Разработка на потребителски интерфейс за отразяване на личен график и присъствена форма. Отваряне на досието от прозореца графици и оцветяване на колоните за неработни дни.</t>
+  </si>
+  <si>
+    <t>Корекции по функционалността за редакция на екипи</t>
+  </si>
+  <si>
+    <t>Корекции по различни функционалности, задаване на работно време и списък от слъжности за вяско от сменните звена.</t>
   </si>
 </sst>
 </file>
@@ -687,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N88"/>
+  <dimension ref="A1:N94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2189,32 +2201,64 @@
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="1"/>
+      <c r="A82" s="1">
+        <v>42450</v>
+      </c>
       <c r="B82" s="2"/>
-      <c r="C82" s="2"/>
-      <c r="D82" s="2"/>
-      <c r="E82" s="2"/>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="1"/>
+      <c r="C82" s="2">
+        <v>4</v>
+      </c>
+      <c r="D82" s="2">
+        <v>200</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>42451</v>
+      </c>
       <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
-      <c r="D83" s="2"/>
-      <c r="E83" s="2"/>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="1"/>
+      <c r="C83" s="2">
+        <v>2</v>
+      </c>
+      <c r="D83" s="2">
+        <v>100</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>42452</v>
+      </c>
       <c r="B84" s="2"/>
-      <c r="C84" s="2"/>
-      <c r="D84" s="2"/>
-      <c r="E84" s="2"/>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
+      <c r="C84" s="2">
+        <v>4</v>
+      </c>
+      <c r="D84" s="2">
+        <v>200</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>42453</v>
+      </c>
       <c r="B85" s="2"/>
-      <c r="C85" s="2"/>
-      <c r="D85" s="2"/>
-      <c r="E85" s="2"/>
+      <c r="C85" s="2">
+        <v>6</v>
+      </c>
+      <c r="D85" s="2">
+        <v>300</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
@@ -2230,15 +2274,57 @@
       <c r="D87" s="2"/>
       <c r="E87" s="2"/>
     </row>
-    <row r="88" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A88" s="3" t="s">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="1"/>
+      <c r="B88" s="2"/>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2"/>
+      <c r="E88" s="2"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="1"/>
+      <c r="B89" s="2"/>
+      <c r="C89" s="2"/>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="1"/>
+      <c r="B90" s="2"/>
+      <c r="C90" s="2"/>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="1"/>
+      <c r="B91" s="2"/>
+      <c r="C91" s="2"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="1"/>
+      <c r="B92" s="2"/>
+      <c r="C92" s="2"/>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="1"/>
+      <c r="B93" s="2"/>
+      <c r="C93" s="2"/>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2"/>
+    </row>
+    <row r="94" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A94" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B88" s="4"/>
-      <c r="C88" s="4"/>
-      <c r="D88" s="3">
-        <f>SUM(D2:D81)</f>
-        <v>5950</v>
+      <c r="B94" s="4"/>
+      <c r="C94" s="4"/>
+      <c r="D94" s="3">
+        <f>SUM(D2:D85)</f>
+        <v>6750</v>
       </c>
     </row>
   </sheetData>

</xml_diff>